<commit_message>
class based implementation checked
</commit_message>
<xml_diff>
--- a/config/test.xlsx
+++ b/config/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schir\OneDrive\Studium\34_Github\PyPowerSim\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E686557-A49E-4559-B444-CD7908C3F492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE0971F-D144-4605-B213-AD86875538F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -484,9 +484,6 @@
     <t>PWM</t>
   </si>
   <si>
-    <t>SV</t>
-  </si>
-  <si>
     <t>DE</t>
   </si>
   <si>
@@ -782,7 +779,10 @@
     <t>none</t>
   </si>
   <si>
-    <t>B2</t>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>B6</t>
   </si>
 </sst>
 </file>
@@ -1713,7 +1713,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1792,7 +1792,7 @@
         <v>39</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>23</v>
@@ -1810,7 +1810,7 @@
         <v>40</v>
       </c>
       <c r="E5" s="29">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>29</v>
@@ -2240,8 +2240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799FBFCB-8244-4B83-8CC9-EBD2890613E5}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2537,8 +2537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245B3F0A-B85A-4162-A12D-AC7176B54015}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2570,19 +2570,19 @@
     </row>
     <row r="2" spans="1:6" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>143</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>144</v>
+        <v>235</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>23</v>
@@ -2590,19 +2590,19 @@
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="42" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>143</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>133</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>23</v>
@@ -2610,19 +2610,19 @@
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B4" s="35" t="s">
         <v>143</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>134</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>23</v>
@@ -2630,19 +2630,19 @@
     </row>
     <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B5" s="35" t="s">
         <v>143</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>135</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>23</v>
@@ -2650,13 +2650,13 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>143</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>43</v>
@@ -2670,13 +2670,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B7" s="35" t="s">
         <v>143</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>136</v>
@@ -2690,13 +2690,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B8" s="35" t="s">
         <v>143</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>137</v>
@@ -2716,7 +2716,7 @@
         <v>143</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>138</v>
@@ -2730,13 +2730,13 @@
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B10" s="35" t="s">
         <v>143</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>139</v>
@@ -2754,7 +2754,7 @@
         <v>143</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>140</v>
@@ -2768,13 +2768,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="42" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B12" s="35" t="s">
         <v>143</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>28</v>
@@ -2788,19 +2788,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B13" s="35" t="s">
         <v>143</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>141</v>
       </c>
       <c r="E13" s="50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>23</v>
@@ -2808,19 +2808,19 @@
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B14" s="36" t="s">
         <v>143</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>142</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>23</v>
@@ -2828,19 +2828,19 @@
     </row>
     <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="41" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>23</v>
@@ -2848,16 +2848,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E16" s="12">
         <v>1050</v>
@@ -2868,16 +2868,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E17" s="12">
         <v>0</v>
@@ -2888,16 +2888,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E18" s="12">
         <v>100</v>
@@ -2908,16 +2908,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E19" s="12">
         <v>1</v>
@@ -2928,16 +2928,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E20" s="12">
         <v>0.1</v>
@@ -2948,16 +2948,16 @@
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="43" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E21" s="30">
         <v>1</v>
@@ -2968,19 +2968,19 @@
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="41" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>23</v>
@@ -2988,19 +2988,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>23</v>
@@ -3008,19 +3008,19 @@
     </row>
     <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>23</v>
@@ -3028,16 +3028,16 @@
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E25" s="12">
         <v>0</v>
@@ -3048,16 +3048,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E26" s="12">
         <v>1</v>
@@ -3068,16 +3068,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="42" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E27" s="12">
         <v>1</v>
@@ -3088,19 +3088,19 @@
     </row>
     <row r="28" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>23</v>
@@ -3108,16 +3108,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>99</v>
@@ -3128,16 +3128,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="42" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E30" s="12">
         <v>1</v>
@@ -3148,16 +3148,16 @@
     </row>
     <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="43" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E31" s="30">
         <v>1</v>
@@ -3168,16 +3168,16 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E32" s="23">
         <v>1</v>
@@ -3191,13 +3191,13 @@
         <v>50</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E33" s="30">
         <v>0</v>

</xml_diff>

<commit_message>
Final class based implementation
</commit_message>
<xml_diff>
--- a/config/test.xlsx
+++ b/config/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schir\OneDrive\Studium\34_Github\PyPowerSim\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE0971F-D144-4605-B213-AD86875538F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EBD730-98F9-43DC-B1B0-7369BCBEA9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -782,7 +782,7 @@
     <t>CB</t>
   </si>
   <si>
-    <t>B6</t>
+    <t>B2</t>
   </si>
 </sst>
 </file>
@@ -2240,7 +2240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799FBFCB-8244-4B83-8CC9-EBD2890613E5}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2537,7 +2537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245B3F0A-B85A-4162-A12D-AC7176B54015}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
First implementation closed loop
</commit_message>
<xml_diff>
--- a/config/test.xlsx
+++ b/config/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schir\OneDrive\Studium\34_Github\PyPowerSim\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4834D35A-4E03-4C7F-8361-85686AB8F80C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33280999-6317-40BC-B75D-4DD912F4CABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7360" activeTab="3" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -779,7 +779,7 @@
     <t>CB</t>
   </si>
   <si>
-    <t>B6</t>
+    <t>B2</t>
   </si>
 </sst>
 </file>
@@ -1710,7 +1710,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1807,7 +1807,7 @@
         <v>40</v>
       </c>
       <c r="E5" s="29">
-        <v>100000</v>
+        <v>500000</v>
       </c>
       <c r="F5" s="24" t="s">
         <v>29</v>
@@ -2237,7 +2237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799FBFCB-8244-4B83-8CC9-EBD2890613E5}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -2534,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245B3F0A-B85A-4162-A12D-AC7176B54015}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2777,7 +2777,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="12">
-        <v>1050</v>
+        <v>5000</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>29</v>
@@ -2857,7 +2857,7 @@
         <v>160</v>
       </c>
       <c r="E16" s="12">
-        <v>1050</v>
+        <v>5000</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Fixing bug in reference generation
</commit_message>
<xml_diff>
--- a/config/test.xlsx
+++ b/config/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schir\OneDrive\Studium\34_Github\PyPowerSim\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FD28D4-14B1-460F-AF5A-23DF8D0108DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B91C0F-5E8B-4559-8332-4357B5B6080D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -388,9 +388,6 @@
     <t>fel</t>
   </si>
   <si>
-    <t>sin</t>
-  </si>
-  <si>
     <t>(B2): half bridge, 
 (B4): full bridge, 
 (B6): two-level three phase converter</t>
@@ -780,6 +777,9 @@
   </si>
   <si>
     <t>B2</t>
+  </si>
+  <si>
+    <t>sin</t>
   </si>
 </sst>
 </file>
@@ -1709,7 +1709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CAB857B-5D2E-4BE1-B462-B4B5EEAA4370}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -1904,7 +1904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86190CFD-1D2B-4FE4-A04E-A3C453840C86}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2237,7 +2237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799FBFCB-8244-4B83-8CC9-EBD2890613E5}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -2270,17 +2270,17 @@
     </row>
     <row r="2" spans="1:6" ht="44.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="45"/>
       <c r="C2" s="46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D2" s="47" t="s">
         <v>98</v>
       </c>
       <c r="E2" s="48" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F2" s="49" t="s">
         <v>23</v>
@@ -2290,7 +2290,7 @@
       <c r="A3" s="31"/>
       <c r="B3" s="20"/>
       <c r="C3" s="21" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>100</v>
@@ -2306,7 +2306,7 @@
       <c r="A4" s="32"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>101</v>
@@ -2322,7 +2322,7 @@
       <c r="A5" s="32"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>102</v>
@@ -2331,14 +2331,14 @@
         <v>1E-3</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="32"/>
       <c r="B6" s="10"/>
       <c r="C6" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>103</v>
@@ -2347,14 +2347,14 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="32"/>
       <c r="B7" s="10"/>
       <c r="C7" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>104</v>
@@ -2370,7 +2370,7 @@
       <c r="A8" s="32"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>105</v>
@@ -2386,7 +2386,7 @@
       <c r="A9" s="32"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>106</v>
@@ -2395,14 +2395,14 @@
         <v>1E-3</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="32"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>107</v>
@@ -2411,14 +2411,14 @@
         <v>1E-3</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="32"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>108</v>
@@ -2434,7 +2434,7 @@
       <c r="A12" s="32"/>
       <c r="B12" s="10"/>
       <c r="C12" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>109</v>
@@ -2443,14 +2443,14 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="32"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>110</v>
@@ -2466,7 +2466,7 @@
       <c r="A14" s="32"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>111</v>
@@ -2482,13 +2482,13 @@
       <c r="A15" s="32"/>
       <c r="B15" s="10"/>
       <c r="C15" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>112</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>114</v>
+        <v>235</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>23</v>
@@ -2498,7 +2498,7 @@
       <c r="A16" s="33"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>113</v>
@@ -2534,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245B3F0A-B85A-4162-A12D-AC7176B54015}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2567,19 +2567,19 @@
     </row>
     <row r="2" spans="1:6" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>23</v>
@@ -2587,19 +2587,19 @@
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B3" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>143</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>144</v>
       </c>
       <c r="F3" s="14" t="s">
         <v>23</v>
@@ -2607,19 +2607,19 @@
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="42" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F4" s="14" t="s">
         <v>23</v>
@@ -2627,19 +2627,19 @@
     </row>
     <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>23</v>
@@ -2647,13 +2647,13 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>43</v>
@@ -2667,16 +2667,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E7" s="12">
         <v>0</v>
@@ -2687,16 +2687,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E8" s="12">
         <v>0</v>
@@ -2710,13 +2710,13 @@
         <v>26</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E9" s="12">
         <v>1</v>
@@ -2727,16 +2727,16 @@
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E10" s="12">
         <v>1</v>
@@ -2748,13 +2748,13 @@
     <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="42"/>
       <c r="B11" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E11" s="12">
         <v>0</v>
@@ -2765,19 +2765,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E12" s="12">
-        <v>2000</v>
+        <v>1050</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>29</v>
@@ -2785,19 +2785,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="42" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E13" s="50" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>23</v>
@@ -2805,19 +2805,19 @@
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="43" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>23</v>
@@ -2825,19 +2825,19 @@
     </row>
     <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="41" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>23</v>
@@ -2845,19 +2845,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E16" s="12">
-        <v>2000</v>
+        <v>5000</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>29</v>
@@ -2865,16 +2865,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E17" s="12">
         <v>0</v>
@@ -2885,16 +2885,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E18" s="12">
         <v>100</v>
@@ -2905,16 +2905,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E19" s="12">
         <v>1</v>
@@ -2925,16 +2925,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B20" s="35" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E20" s="12">
         <v>0.1</v>
@@ -2945,16 +2945,16 @@
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E21" s="30">
         <v>1</v>
@@ -2965,19 +2965,19 @@
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B22" s="34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>23</v>
@@ -2985,19 +2985,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B23" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>23</v>
@@ -3005,19 +3005,19 @@
     </row>
     <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>23</v>
@@ -3025,16 +3025,16 @@
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B25" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E25" s="12">
         <v>0</v>
@@ -3045,16 +3045,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E26" s="12">
         <v>1</v>
@@ -3065,16 +3065,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B27" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E27" s="12">
         <v>1</v>
@@ -3085,19 +3085,19 @@
     </row>
     <row r="28" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="42" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B28" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>23</v>
@@ -3105,16 +3105,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>99</v>
@@ -3125,16 +3125,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B30" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E30" s="12">
         <v>1</v>
@@ -3145,16 +3145,16 @@
     </row>
     <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="43" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B31" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E31" s="30">
         <v>1</v>
@@ -3165,16 +3165,16 @@
     </row>
     <row r="32" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B32" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E32" s="23">
         <v>1</v>
@@ -3188,13 +3188,13 @@
         <v>50</v>
       </c>
       <c r="B33" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E33" s="30">
         <v>0</v>

</xml_diff>

<commit_message>
Generalised closed loop approach
The approach works for the B2 bridge and needs to be extended for the other classes. The plotting needs to be added as well.
</commit_message>
<xml_diff>
--- a/config/test.xlsx
+++ b/config/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schir\OneDrive\Studium\34_Github\PyPowerSim\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B91C0F-5E8B-4559-8332-4357B5B6080D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03F486A-451C-44B7-9FEE-9B9765F5BCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{DB7D2548-4471-4992-93B1-3EC0BA66F7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="2" r:id="rId1"/>
@@ -556,9 +556,6 @@
     <t>Ther</t>
   </si>
   <si>
-    <t>PI</t>
-  </si>
-  <si>
     <t>tab</t>
   </si>
   <si>
@@ -780,6 +777,9 @@
   </si>
   <si>
     <t>sin</t>
+  </si>
+  <si>
+    <t>HY</t>
   </si>
 </sst>
 </file>
@@ -2237,8 +2237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{799FBFCB-8244-4B83-8CC9-EBD2890613E5}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2280,7 +2280,7 @@
         <v>98</v>
       </c>
       <c r="E2" s="48" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F2" s="49" t="s">
         <v>23</v>
@@ -2424,7 +2424,7 @@
         <v>108</v>
       </c>
       <c r="E11" s="13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>24</v>
@@ -2488,7 +2488,7 @@
         <v>112</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>23</v>
@@ -2534,8 +2534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245B3F0A-B85A-4162-A12D-AC7176B54015}">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2567,19 +2567,19 @@
     </row>
     <row r="2" spans="1:6" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B2" s="34" t="s">
         <v>142</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D2" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F2" s="24" t="s">
         <v>23</v>
@@ -2587,13 +2587,13 @@
     </row>
     <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="42" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>142</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>132</v>
@@ -2607,13 +2607,13 @@
     </row>
     <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B4" s="35" t="s">
         <v>142</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>133</v>
@@ -2627,13 +2627,13 @@
     </row>
     <row r="5" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="42" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B5" s="35" t="s">
         <v>142</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>134</v>
@@ -2647,13 +2647,13 @@
     </row>
     <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="42" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>142</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>43</v>
@@ -2667,13 +2667,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="42" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B7" s="35" t="s">
         <v>142</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>135</v>
@@ -2687,13 +2687,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="42" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B8" s="35" t="s">
         <v>142</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>136</v>
@@ -2713,7 +2713,7 @@
         <v>142</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>137</v>
@@ -2727,13 +2727,13 @@
     </row>
     <row r="10" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="42" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B10" s="35" t="s">
         <v>142</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>138</v>
@@ -2751,7 +2751,7 @@
         <v>142</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>139</v>
@@ -2765,13 +2765,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B12" s="35" t="s">
         <v>142</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>28</v>
@@ -2785,19 +2785,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="42" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B13" s="35" t="s">
         <v>142</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>140</v>
       </c>
       <c r="E13" s="50" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>23</v>
@@ -2805,13 +2805,13 @@
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="43" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B14" s="36" t="s">
         <v>142</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>141</v>
@@ -2825,19 +2825,19 @@
     </row>
     <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="41" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B15" s="34" t="s">
         <v>165</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D15" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>168</v>
+        <v>235</v>
       </c>
       <c r="F15" s="24" t="s">
         <v>23</v>
@@ -2845,13 +2845,13 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="42" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B16" s="35" t="s">
         <v>165</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>159</v>
@@ -2865,13 +2865,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B17" s="35" t="s">
         <v>165</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>160</v>
@@ -2885,13 +2885,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="42" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B18" s="35" t="s">
         <v>165</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>161</v>
@@ -2905,13 +2905,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B19" s="35" t="s">
         <v>165</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>162</v>
@@ -2925,13 +2925,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B20" s="35" t="s">
         <v>165</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>163</v>
@@ -2945,13 +2945,13 @@
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="43" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B21" s="36" t="s">
         <v>165</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>164</v>
@@ -2965,19 +2965,19 @@
     </row>
     <row r="22" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="41" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B22" s="34" t="s">
         <v>166</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>147</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F22" s="24" t="s">
         <v>23</v>
@@ -2985,19 +2985,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="42" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B23" s="35" t="s">
         <v>166</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>148</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F23" s="14" t="s">
         <v>23</v>
@@ -3005,19 +3005,19 @@
     </row>
     <row r="24" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B24" s="35" t="s">
         <v>166</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>149</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>23</v>
@@ -3025,13 +3025,13 @@
     </row>
     <row r="25" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B25" s="35" t="s">
         <v>166</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>150</v>
@@ -3045,13 +3045,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="42" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B26" s="35" t="s">
         <v>166</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>151</v>
@@ -3065,13 +3065,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B27" s="35" t="s">
         <v>166</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>152</v>
@@ -3085,19 +3085,19 @@
     </row>
     <row r="28" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="42" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B28" s="35" t="s">
         <v>166</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>153</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>23</v>
@@ -3105,13 +3105,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B29" s="35" t="s">
         <v>166</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>154</v>
@@ -3125,13 +3125,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="42" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B30" s="35" t="s">
         <v>166</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>155</v>
@@ -3145,13 +3145,13 @@
     </row>
     <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="43" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B31" s="36" t="s">
         <v>166</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>156</v>
@@ -3171,7 +3171,7 @@
         <v>167</v>
       </c>
       <c r="C32" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D32" s="22" t="s">
         <v>157</v>
@@ -3191,7 +3191,7 @@
         <v>167</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>158</v>

</xml_diff>